<commit_message>
added new excel data
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E1DA82-EDBC-47E1-9C48-53FD10E70EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Admin</t>
   </si>
@@ -59,11 +60,14 @@
   <si>
     <t>Nitesh_50</t>
   </si>
+  <si>
+    <t>Admin1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -409,20 +413,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -432,22 +444,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -461,7 +473,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -476,7 +488,7 @@
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -490,7 +502,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -511,24 +523,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added new excel data1
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E1DA82-EDBC-47E1-9C48-53FD10E70EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8E3FF0-F657-4265-8CE6-4E8ABEBEF1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>Admin</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Admin1</t>
+  </si>
+  <si>
+    <t>Admin3</t>
   </si>
 </sst>
 </file>
@@ -414,11 +417,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -435,6 +436,14 @@
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>